<commit_message>
cleaning up minor items and last upload to Test ERP
</commit_message>
<xml_diff>
--- a/OpsAndMats/M188.xlsx
+++ b/OpsAndMats/M188.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eclark.LABTESTING\Documents\ERP Notes\Phase2_BOM\OpsAndMats\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D961B28D-A6B1-41AA-A6E5-6288E373CCBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
     <sheet name="Operations" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1034,8 +1028,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1098,14 +1092,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1152,7 +1138,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1184,27 +1170,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1236,24 +1204,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1429,16 +1379,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AQ244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A212" workbookViewId="0">
-      <selection activeCell="U245" sqref="U245"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1569,7 +1517,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1652,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1735,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1818,7 +1766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1901,7 +1849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -1984,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -2067,7 +2015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -2150,7 +2098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -2233,7 +2181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -2316,7 +2264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -2399,7 +2347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2482,7 +2430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2565,7 +2513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -2648,7 +2596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2731,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -2814,7 +2762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2897,7 +2845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -2980,7 +2928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -3063,7 +3011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -3146,7 +3094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -3229,7 +3177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -3312,7 +3260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -3395,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -3478,7 +3426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -3561,7 +3509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -3644,7 +3592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:43">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -3727,7 +3675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -3810,7 +3758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -3893,7 +3841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -3976,7 +3924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -4059,7 +4007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -4142,7 +4090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -4225,7 +4173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -4308,7 +4256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -4391,7 +4339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:43">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -4474,7 +4422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:43">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -4557,7 +4505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:43">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -4640,7 +4588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:43">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -4723,7 +4671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:43">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -4806,7 +4754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:43">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -4889,7 +4837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:43">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -4972,7 +4920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:43">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -5055,7 +5003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:43">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -5138,7 +5086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:43">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -5221,7 +5169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:43">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -5304,7 +5252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:43">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -5387,7 +5335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:43">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -5470,7 +5418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:43">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -5553,7 +5501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:43">
       <c r="A50" t="s">
         <v>46</v>
       </c>
@@ -5636,7 +5584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:43">
       <c r="A51" t="s">
         <v>46</v>
       </c>
@@ -5719,7 +5667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:43">
       <c r="A52" t="s">
         <v>46</v>
       </c>
@@ -5802,7 +5750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:43">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -5885,7 +5833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:43">
       <c r="A54" t="s">
         <v>46</v>
       </c>
@@ -5968,7 +5916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:43">
       <c r="A55" t="s">
         <v>46</v>
       </c>
@@ -6051,7 +5999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:43">
       <c r="A56" t="s">
         <v>46</v>
       </c>
@@ -6134,7 +6082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:43">
       <c r="A57" t="s">
         <v>46</v>
       </c>
@@ -6217,7 +6165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:43">
       <c r="A58" t="s">
         <v>46</v>
       </c>
@@ -6300,7 +6248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:43">
       <c r="A59" t="s">
         <v>47</v>
       </c>
@@ -6383,7 +6331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:43">
       <c r="A60" t="s">
         <v>47</v>
       </c>
@@ -6466,7 +6414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:43">
       <c r="A61" t="s">
         <v>47</v>
       </c>
@@ -6549,7 +6497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:43">
       <c r="A62" t="s">
         <v>47</v>
       </c>
@@ -6632,7 +6580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:43">
       <c r="A63" t="s">
         <v>47</v>
       </c>
@@ -6715,7 +6663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:43">
       <c r="A64" t="s">
         <v>47</v>
       </c>
@@ -6798,7 +6746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:43">
       <c r="A65" t="s">
         <v>47</v>
       </c>
@@ -6881,7 +6829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:43">
       <c r="A66" t="s">
         <v>47</v>
       </c>
@@ -6964,7 +6912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:43">
       <c r="A67" t="s">
         <v>47</v>
       </c>
@@ -7047,7 +6995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:43">
       <c r="A68" t="s">
         <v>47</v>
       </c>
@@ -7130,7 +7078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:43">
       <c r="A69" t="s">
         <v>48</v>
       </c>
@@ -7213,7 +7161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:43">
       <c r="A70" t="s">
         <v>48</v>
       </c>
@@ -7296,7 +7244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:43">
       <c r="A71" t="s">
         <v>48</v>
       </c>
@@ -7379,7 +7327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:43">
       <c r="A72" t="s">
         <v>48</v>
       </c>
@@ -7462,7 +7410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:43">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -7545,7 +7493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:43">
       <c r="A74" t="s">
         <v>48</v>
       </c>
@@ -7628,7 +7576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:43">
       <c r="A75" t="s">
         <v>48</v>
       </c>
@@ -7711,7 +7659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:43">
       <c r="A76" t="s">
         <v>48</v>
       </c>
@@ -7794,7 +7742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:43">
       <c r="A77" t="s">
         <v>48</v>
       </c>
@@ -7877,7 +7825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:43">
       <c r="A78" t="s">
         <v>48</v>
       </c>
@@ -7960,7 +7908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:43">
       <c r="A79" t="s">
         <v>49</v>
       </c>
@@ -8043,7 +7991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:43">
       <c r="A80" t="s">
         <v>49</v>
       </c>
@@ -8126,7 +8074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:43">
       <c r="A81" t="s">
         <v>49</v>
       </c>
@@ -8209,7 +8157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:43">
       <c r="A82" t="s">
         <v>49</v>
       </c>
@@ -8292,7 +8240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:43">
       <c r="A83" t="s">
         <v>49</v>
       </c>
@@ -8375,7 +8323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:43">
       <c r="A84" t="s">
         <v>49</v>
       </c>
@@ -8458,7 +8406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:43">
       <c r="A85" t="s">
         <v>49</v>
       </c>
@@ -8541,7 +8489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:43">
       <c r="A86" t="s">
         <v>49</v>
       </c>
@@ -8624,7 +8572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:43">
       <c r="A87" t="s">
         <v>49</v>
       </c>
@@ -8707,7 +8655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:43">
       <c r="A88" t="s">
         <v>49</v>
       </c>
@@ -8790,7 +8738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:43">
       <c r="A89" t="s">
         <v>49</v>
       </c>
@@ -8873,7 +8821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:43">
       <c r="A90" t="s">
         <v>49</v>
       </c>
@@ -8956,7 +8904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:43">
       <c r="A91" t="s">
         <v>49</v>
       </c>
@@ -9039,7 +8987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:43">
       <c r="A92" t="s">
         <v>49</v>
       </c>
@@ -9122,7 +9070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:43">
       <c r="A93" t="s">
         <v>49</v>
       </c>
@@ -9205,7 +9153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:43">
       <c r="A94" t="s">
         <v>49</v>
       </c>
@@ -9288,7 +9236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:43">
       <c r="A95" t="s">
         <v>49</v>
       </c>
@@ -9371,7 +9319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:43">
       <c r="A96" t="s">
         <v>49</v>
       </c>
@@ -9454,7 +9402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:43">
       <c r="A97" t="s">
         <v>49</v>
       </c>
@@ -9537,7 +9485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:43">
       <c r="A98" t="s">
         <v>49</v>
       </c>
@@ -9620,7 +9568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:43">
       <c r="A99" t="s">
         <v>49</v>
       </c>
@@ -9703,7 +9651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:43">
       <c r="A100" t="s">
         <v>49</v>
       </c>
@@ -9786,7 +9734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:43">
       <c r="A101" t="s">
         <v>49</v>
       </c>
@@ -9869,7 +9817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:43">
       <c r="A102" t="s">
         <v>49</v>
       </c>
@@ -9952,7 +9900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:43">
       <c r="A103" t="s">
         <v>49</v>
       </c>
@@ -10035,7 +9983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:43">
       <c r="A104" t="s">
         <v>49</v>
       </c>
@@ -10118,7 +10066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:43">
       <c r="A105" t="s">
         <v>49</v>
       </c>
@@ -10201,7 +10149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:43">
       <c r="A106" t="s">
         <v>49</v>
       </c>
@@ -10284,7 +10232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:43">
       <c r="A107" t="s">
         <v>49</v>
       </c>
@@ -10367,7 +10315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:43">
       <c r="A108" t="s">
         <v>49</v>
       </c>
@@ -10450,7 +10398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:43">
       <c r="A109" t="s">
         <v>49</v>
       </c>
@@ -10533,7 +10481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:43">
       <c r="A110" t="s">
         <v>49</v>
       </c>
@@ -10616,7 +10564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:43">
       <c r="A111" t="s">
         <v>49</v>
       </c>
@@ -10699,7 +10647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:43">
       <c r="A112" t="s">
         <v>49</v>
       </c>
@@ -10782,7 +10730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:43">
       <c r="A113" t="s">
         <v>50</v>
       </c>
@@ -10865,7 +10813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:43">
       <c r="A114" t="s">
         <v>50</v>
       </c>
@@ -10948,7 +10896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:43">
       <c r="A115" t="s">
         <v>50</v>
       </c>
@@ -11031,7 +10979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:43">
       <c r="A116" t="s">
         <v>50</v>
       </c>
@@ -11114,7 +11062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:43">
       <c r="A117" t="s">
         <v>50</v>
       </c>
@@ -11197,7 +11145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:43">
       <c r="A118" t="s">
         <v>50</v>
       </c>
@@ -11280,7 +11228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:43">
       <c r="A119" t="s">
         <v>50</v>
       </c>
@@ -11363,7 +11311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:43">
       <c r="A120" t="s">
         <v>51</v>
       </c>
@@ -11446,7 +11394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:43">
       <c r="A121" t="s">
         <v>51</v>
       </c>
@@ -11529,7 +11477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:43">
       <c r="A122" t="s">
         <v>51</v>
       </c>
@@ -11612,7 +11560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:43">
       <c r="A123" t="s">
         <v>51</v>
       </c>
@@ -11695,7 +11643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:43">
       <c r="A124" t="s">
         <v>51</v>
       </c>
@@ -11778,7 +11726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:43">
       <c r="A125" t="s">
         <v>51</v>
       </c>
@@ -11861,7 +11809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:43">
       <c r="A126" t="s">
         <v>51</v>
       </c>
@@ -11944,7 +11892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:43">
       <c r="A127" t="s">
         <v>52</v>
       </c>
@@ -12027,7 +11975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:43">
       <c r="A128" t="s">
         <v>52</v>
       </c>
@@ -12110,7 +12058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:43">
       <c r="A129" t="s">
         <v>52</v>
       </c>
@@ -12193,7 +12141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:43">
       <c r="A130" t="s">
         <v>52</v>
       </c>
@@ -12276,7 +12224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:43">
       <c r="A131" t="s">
         <v>52</v>
       </c>
@@ -12359,7 +12307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:43">
       <c r="A132" t="s">
         <v>52</v>
       </c>
@@ -12442,7 +12390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:43">
       <c r="A133" t="s">
         <v>52</v>
       </c>
@@ -12525,7 +12473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:43">
       <c r="A134" t="s">
         <v>53</v>
       </c>
@@ -12608,7 +12556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:43">
       <c r="A135" t="s">
         <v>53</v>
       </c>
@@ -12691,7 +12639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:43">
       <c r="A136" t="s">
         <v>53</v>
       </c>
@@ -12774,7 +12722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:43">
       <c r="A137" t="s">
         <v>53</v>
       </c>
@@ -12857,7 +12805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:43">
       <c r="A138" t="s">
         <v>53</v>
       </c>
@@ -12940,7 +12888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:43">
       <c r="A139" t="s">
         <v>53</v>
       </c>
@@ -13023,7 +12971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:43">
       <c r="A140" t="s">
         <v>53</v>
       </c>
@@ -13106,7 +13054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:43">
       <c r="A141" t="s">
         <v>53</v>
       </c>
@@ -13189,7 +13137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:43">
       <c r="A142" t="s">
         <v>53</v>
       </c>
@@ -13272,7 +13220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:43">
       <c r="A143" t="s">
         <v>53</v>
       </c>
@@ -13355,7 +13303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:43">
       <c r="A144" t="s">
         <v>53</v>
       </c>
@@ -13438,7 +13386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:43">
       <c r="A145" t="s">
         <v>53</v>
       </c>
@@ -13521,7 +13469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:43">
       <c r="A146" t="s">
         <v>53</v>
       </c>
@@ -13604,7 +13552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:43">
       <c r="A147" t="s">
         <v>53</v>
       </c>
@@ -13687,7 +13635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:43">
       <c r="A148" t="s">
         <v>53</v>
       </c>
@@ -13770,7 +13718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:43">
       <c r="A149" t="s">
         <v>53</v>
       </c>
@@ -13853,7 +13801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:43">
       <c r="A150" t="s">
         <v>54</v>
       </c>
@@ -13936,7 +13884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:43">
       <c r="A151" t="s">
         <v>54</v>
       </c>
@@ -14019,7 +13967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:43">
       <c r="A152" t="s">
         <v>54</v>
       </c>
@@ -14102,7 +14050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:43">
       <c r="A153" t="s">
         <v>54</v>
       </c>
@@ -14185,7 +14133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:43">
       <c r="A154" t="s">
         <v>54</v>
       </c>
@@ -14268,7 +14216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:43">
       <c r="A155" t="s">
         <v>54</v>
       </c>
@@ -14351,7 +14299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:43">
       <c r="A156" t="s">
         <v>54</v>
       </c>
@@ -14434,7 +14382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:43">
       <c r="A157" t="s">
         <v>54</v>
       </c>
@@ -14517,7 +14465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:43">
       <c r="A158" t="s">
         <v>54</v>
       </c>
@@ -14600,7 +14548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:43">
       <c r="A159" t="s">
         <v>54</v>
       </c>
@@ -14683,7 +14631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:43">
       <c r="A160" t="s">
         <v>54</v>
       </c>
@@ -14766,7 +14714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:43">
       <c r="A161" t="s">
         <v>54</v>
       </c>
@@ -14849,7 +14797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:43">
       <c r="A162" t="s">
         <v>54</v>
       </c>
@@ -14932,7 +14880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:43">
       <c r="A163" t="s">
         <v>54</v>
       </c>
@@ -15015,7 +14963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:43">
       <c r="A164" t="s">
         <v>54</v>
       </c>
@@ -15098,7 +15046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:43">
       <c r="A165" t="s">
         <v>54</v>
       </c>
@@ -15181,7 +15129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:43">
       <c r="A166" t="s">
         <v>54</v>
       </c>
@@ -15264,7 +15212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:43">
       <c r="A167" t="s">
         <v>54</v>
       </c>
@@ -15347,7 +15295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:43">
       <c r="A168" t="s">
         <v>54</v>
       </c>
@@ -15430,7 +15378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:43">
       <c r="A169" t="s">
         <v>54</v>
       </c>
@@ -15513,7 +15461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:43">
       <c r="A170" t="s">
         <v>54</v>
       </c>
@@ -15596,7 +15544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:43">
       <c r="A171" t="s">
         <v>55</v>
       </c>
@@ -15679,7 +15627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:43">
       <c r="A172" t="s">
         <v>55</v>
       </c>
@@ -15762,7 +15710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:43">
       <c r="A173" t="s">
         <v>55</v>
       </c>
@@ -15845,7 +15793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:43">
       <c r="A174" t="s">
         <v>55</v>
       </c>
@@ -15928,7 +15876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:43">
       <c r="A175" t="s">
         <v>55</v>
       </c>
@@ -16011,7 +15959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:43">
       <c r="A176" t="s">
         <v>55</v>
       </c>
@@ -16094,7 +16042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:43">
       <c r="A177" t="s">
         <v>55</v>
       </c>
@@ -16177,7 +16125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:43">
       <c r="A178" t="s">
         <v>55</v>
       </c>
@@ -16260,7 +16208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:43">
       <c r="A179" t="s">
         <v>55</v>
       </c>
@@ -16343,7 +16291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:43">
       <c r="A180" t="s">
         <v>55</v>
       </c>
@@ -16426,7 +16374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:43">
       <c r="A181" t="s">
         <v>55</v>
       </c>
@@ -16509,7 +16457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:43">
       <c r="A182" t="s">
         <v>55</v>
       </c>
@@ -16592,7 +16540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:43">
       <c r="A183" t="s">
         <v>55</v>
       </c>
@@ -16675,7 +16623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:43">
       <c r="A184" t="s">
         <v>55</v>
       </c>
@@ -16758,7 +16706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:43">
       <c r="A185" t="s">
         <v>55</v>
       </c>
@@ -16841,7 +16789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:43">
       <c r="A186" t="s">
         <v>55</v>
       </c>
@@ -16924,7 +16872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:43">
       <c r="A187" t="s">
         <v>55</v>
       </c>
@@ -17007,7 +16955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:43">
       <c r="A188" t="s">
         <v>56</v>
       </c>
@@ -17090,7 +17038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:43">
       <c r="A189" t="s">
         <v>57</v>
       </c>
@@ -17173,7 +17121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:43">
       <c r="A190" t="s">
         <v>58</v>
       </c>
@@ -17256,7 +17204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:43">
       <c r="A191" t="s">
         <v>58</v>
       </c>
@@ -17339,7 +17287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:43">
       <c r="A192" t="s">
         <v>58</v>
       </c>
@@ -17422,7 +17370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:43">
       <c r="A193" t="s">
         <v>58</v>
       </c>
@@ -17505,7 +17453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:43">
       <c r="A194" t="s">
         <v>59</v>
       </c>
@@ -17588,7 +17536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:43">
       <c r="A195" t="s">
         <v>60</v>
       </c>
@@ -17671,7 +17619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:43">
       <c r="A196" t="s">
         <v>61</v>
       </c>
@@ -17754,7 +17702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:43">
       <c r="A197" t="s">
         <v>62</v>
       </c>
@@ -17837,7 +17785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:43">
       <c r="A198" t="s">
         <v>63</v>
       </c>
@@ -17920,7 +17868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:43">
       <c r="A199" t="s">
         <v>63</v>
       </c>
@@ -18003,7 +17951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:43">
       <c r="A200" t="s">
         <v>64</v>
       </c>
@@ -18086,7 +18034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:43">
       <c r="A201" t="s">
         <v>64</v>
       </c>
@@ -18169,7 +18117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:43">
       <c r="A202" t="s">
         <v>65</v>
       </c>
@@ -18252,7 +18200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:43">
       <c r="A203" t="s">
         <v>65</v>
       </c>
@@ -18335,7 +18283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:43">
       <c r="A204" t="s">
         <v>66</v>
       </c>
@@ -18418,7 +18366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:43">
       <c r="A205" t="s">
         <v>66</v>
       </c>
@@ -18501,7 +18449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:43">
       <c r="A206" t="s">
         <v>67</v>
       </c>
@@ -18584,7 +18532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:43">
       <c r="A207" t="s">
         <v>67</v>
       </c>
@@ -18667,7 +18615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:43">
       <c r="A208" t="s">
         <v>68</v>
       </c>
@@ -18750,7 +18698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:43">
       <c r="A209" t="s">
         <v>68</v>
       </c>
@@ -18833,7 +18781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:43">
       <c r="A210" t="s">
         <v>69</v>
       </c>
@@ -18916,7 +18864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:43">
       <c r="A211" t="s">
         <v>69</v>
       </c>
@@ -18999,7 +18947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:43">
       <c r="A212" t="s">
         <v>70</v>
       </c>
@@ -19082,7 +19030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:43">
       <c r="A213" t="s">
         <v>70</v>
       </c>
@@ -19165,7 +19113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:43">
       <c r="A214" t="s">
         <v>71</v>
       </c>
@@ -19248,7 +19196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:43">
       <c r="A215" t="s">
         <v>71</v>
       </c>
@@ -19331,7 +19279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:43">
       <c r="A216" t="s">
         <v>71</v>
       </c>
@@ -19414,7 +19362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:43">
       <c r="A217" t="s">
         <v>71</v>
       </c>
@@ -19497,7 +19445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:43">
       <c r="A218" t="s">
         <v>71</v>
       </c>
@@ -19580,7 +19528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:43">
       <c r="A219" t="s">
         <v>72</v>
       </c>
@@ -19663,7 +19611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:43">
       <c r="A220" t="s">
         <v>73</v>
       </c>
@@ -19746,7 +19694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:43">
       <c r="A221" t="s">
         <v>74</v>
       </c>
@@ -19829,7 +19777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:43">
       <c r="A222" t="s">
         <v>75</v>
       </c>
@@ -19912,7 +19860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:43">
       <c r="A223" t="s">
         <v>76</v>
       </c>
@@ -19995,7 +19943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:43">
       <c r="A224" t="s">
         <v>76</v>
       </c>
@@ -20078,7 +20026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:43">
       <c r="A225" t="s">
         <v>77</v>
       </c>
@@ -20161,7 +20109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:43">
       <c r="A226" t="s">
         <v>77</v>
       </c>
@@ -20244,7 +20192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:43">
       <c r="A227" t="s">
         <v>78</v>
       </c>
@@ -20327,7 +20275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:43">
       <c r="A228" t="s">
         <v>78</v>
       </c>
@@ -20410,7 +20358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:43">
       <c r="A229" t="s">
         <v>78</v>
       </c>
@@ -20493,7 +20441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:43">
       <c r="A230" t="s">
         <v>79</v>
       </c>
@@ -20576,7 +20524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:43">
       <c r="A231" t="s">
         <v>80</v>
       </c>
@@ -20659,7 +20607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:43">
       <c r="A232" t="s">
         <v>81</v>
       </c>
@@ -20742,7 +20690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:43">
       <c r="A233" t="s">
         <v>82</v>
       </c>
@@ -20825,7 +20773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:43">
       <c r="A234" t="s">
         <v>83</v>
       </c>
@@ -20908,7 +20856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:43">
       <c r="A235" t="s">
         <v>83</v>
       </c>
@@ -20991,7 +20939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:43">
       <c r="A236" t="s">
         <v>84</v>
       </c>
@@ -21074,7 +21022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:43">
       <c r="A237" t="s">
         <v>84</v>
       </c>
@@ -21157,7 +21105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:43">
       <c r="A238" t="s">
         <v>85</v>
       </c>
@@ -21240,7 +21188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:43">
       <c r="A239" t="s">
         <v>85</v>
       </c>
@@ -21323,7 +21271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:43">
       <c r="A240" t="s">
         <v>86</v>
       </c>
@@ -21406,7 +21354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:43">
       <c r="A241" t="s">
         <v>86</v>
       </c>
@@ -21489,7 +21437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:43">
       <c r="A242" t="s">
         <v>87</v>
       </c>
@@ -21572,7 +21520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:43">
       <c r="A243" t="s">
         <v>87</v>
       </c>
@@ -21607,7 +21555,7 @@
         <v>8</v>
       </c>
       <c r="S243">
-        <v>6.25E-2</v>
+        <v>0.0625</v>
       </c>
       <c r="T243" t="s">
         <v>277</v>
@@ -21655,7 +21603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:43">
       <c r="A244" t="s">
         <v>88</v>
       </c>
@@ -21744,16 +21692,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AW116"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD116"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -21902,7 +21848,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -22012,7 +21958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -22122,7 +22068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -22232,7 +22178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -22342,7 +22288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -22452,7 +22398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -22562,7 +22508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -22672,7 +22618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -22782,7 +22728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -22892,7 +22838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -23002,7 +22948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -23112,7 +23058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -23222,7 +23168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -23332,7 +23278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -23442,7 +23388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -23552,7 +23498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -23662,7 +23608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:49">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -23772,7 +23718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:49">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -23882,7 +23828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:49">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -23992,7 +23938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:49">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -24102,7 +24048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:49">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -24212,7 +24158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:49">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -24322,7 +24268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:49">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -24432,7 +24378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:49">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -24542,7 +24488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:49">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -24652,7 +24598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:49">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -24762,7 +24708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:49">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -24872,7 +24818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:49">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -24982,7 +24928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:49">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -25092,7 +25038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:49">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -25202,7 +25148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:49">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -25312,7 +25258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:49">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -25422,7 +25368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:49">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -25532,7 +25478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:49">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -25642,7 +25588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:49">
       <c r="A36" t="s">
         <v>64</v>
       </c>
@@ -25752,7 +25698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:49">
       <c r="A37" t="s">
         <v>64</v>
       </c>
@@ -25862,7 +25808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:49">
       <c r="A38" t="s">
         <v>64</v>
       </c>
@@ -25972,7 +25918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:49">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -26082,7 +26028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:49">
       <c r="A40" t="s">
         <v>65</v>
       </c>
@@ -26192,7 +26138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:49">
       <c r="A41" t="s">
         <v>65</v>
       </c>
@@ -26302,7 +26248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:49">
       <c r="A42" t="s">
         <v>65</v>
       </c>
@@ -26412,7 +26358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:49">
       <c r="A43" t="s">
         <v>66</v>
       </c>
@@ -26522,7 +26468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:49">
       <c r="A44" t="s">
         <v>66</v>
       </c>
@@ -26632,7 +26578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:49">
       <c r="A45" t="s">
         <v>66</v>
       </c>
@@ -26742,7 +26688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:49">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -26852,7 +26798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:49">
       <c r="A47" t="s">
         <v>67</v>
       </c>
@@ -26962,7 +26908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:49">
       <c r="A48" t="s">
         <v>67</v>
       </c>
@@ -27072,7 +27018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:49">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -27182,7 +27128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:49">
       <c r="A50" t="s">
         <v>67</v>
       </c>
@@ -27292,7 +27238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:49">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -27402,7 +27348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:49">
       <c r="A52" t="s">
         <v>68</v>
       </c>
@@ -27512,7 +27458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:49">
       <c r="A53" t="s">
         <v>68</v>
       </c>
@@ -27622,7 +27568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:49">
       <c r="A54" t="s">
         <v>68</v>
       </c>
@@ -27732,7 +27678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:49">
       <c r="A55" t="s">
         <v>69</v>
       </c>
@@ -27842,7 +27788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:49">
       <c r="A56" t="s">
         <v>69</v>
       </c>
@@ -27952,7 +27898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:49">
       <c r="A57" t="s">
         <v>69</v>
       </c>
@@ -28062,7 +28008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:49">
       <c r="A58" t="s">
         <v>69</v>
       </c>
@@ -28172,7 +28118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:49">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -28282,7 +28228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:49">
       <c r="A60" t="s">
         <v>70</v>
       </c>
@@ -28392,7 +28338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:49">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -28502,7 +28448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:49">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -28612,7 +28558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:49">
       <c r="A63" t="s">
         <v>71</v>
       </c>
@@ -28722,7 +28668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:49">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -28832,7 +28778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:49">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -28942,7 +28888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:49">
       <c r="A66" t="s">
         <v>71</v>
       </c>
@@ -29052,7 +28998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:49">
       <c r="A67" t="s">
         <v>71</v>
       </c>
@@ -29162,7 +29108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:49">
       <c r="A68" t="s">
         <v>72</v>
       </c>
@@ -29272,7 +29218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:49">
       <c r="A69" t="s">
         <v>72</v>
       </c>
@@ -29382,7 +29328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:49">
       <c r="A70" t="s">
         <v>73</v>
       </c>
@@ -29492,7 +29438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:49">
       <c r="A71" t="s">
         <v>73</v>
       </c>
@@ -29602,7 +29548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:49">
       <c r="A72" t="s">
         <v>74</v>
       </c>
@@ -29712,7 +29658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:49">
       <c r="A73" t="s">
         <v>75</v>
       </c>
@@ -29822,7 +29768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:49">
       <c r="A74" t="s">
         <v>76</v>
       </c>
@@ -29932,7 +29878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:49">
       <c r="A75" t="s">
         <v>76</v>
       </c>
@@ -30042,7 +29988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:49">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -30152,7 +30098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:49">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -30262,7 +30208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:49">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -30372,7 +30318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:49">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -30482,7 +30428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:49">
       <c r="A80" t="s">
         <v>77</v>
       </c>
@@ -30592,7 +30538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:49">
       <c r="A81" t="s">
         <v>77</v>
       </c>
@@ -30702,7 +30648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:49">
       <c r="A82" t="s">
         <v>78</v>
       </c>
@@ -30812,7 +30758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:49">
       <c r="A83" t="s">
         <v>78</v>
       </c>
@@ -30922,7 +30868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:49">
       <c r="A84" t="s">
         <v>78</v>
       </c>
@@ -31032,7 +30978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:49">
       <c r="A85" t="s">
         <v>79</v>
       </c>
@@ -31142,7 +31088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:49">
       <c r="A86" t="s">
         <v>79</v>
       </c>
@@ -31252,7 +31198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:49">
       <c r="A87" t="s">
         <v>80</v>
       </c>
@@ -31362,7 +31308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:49">
       <c r="A88" t="s">
         <v>80</v>
       </c>
@@ -31472,7 +31418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:49">
       <c r="A89" t="s">
         <v>81</v>
       </c>
@@ -31582,7 +31528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:49">
       <c r="A90" t="s">
         <v>81</v>
       </c>
@@ -31692,7 +31638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:49">
       <c r="A91" t="s">
         <v>81</v>
       </c>
@@ -31802,7 +31748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:49">
       <c r="A92" t="s">
         <v>82</v>
       </c>
@@ -31912,7 +31858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:49">
       <c r="A93" t="s">
         <v>82</v>
       </c>
@@ -32022,7 +31968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:49">
       <c r="A94" t="s">
         <v>82</v>
       </c>
@@ -32132,7 +32078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:49">
       <c r="A95" t="s">
         <v>83</v>
       </c>
@@ -32242,7 +32188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:49">
       <c r="A96" t="s">
         <v>83</v>
       </c>
@@ -32352,7 +32298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:49">
       <c r="A97" t="s">
         <v>83</v>
       </c>
@@ -32462,7 +32408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:49">
       <c r="A98" t="s">
         <v>83</v>
       </c>
@@ -32572,7 +32518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:49">
       <c r="A99" t="s">
         <v>83</v>
       </c>
@@ -32682,7 +32628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:49">
       <c r="A100" t="s">
         <v>84</v>
       </c>
@@ -32792,7 +32738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:49">
       <c r="A101" t="s">
         <v>84</v>
       </c>
@@ -32902,7 +32848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:49">
       <c r="A102" t="s">
         <v>84</v>
       </c>
@@ -33012,7 +32958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:49">
       <c r="A103" t="s">
         <v>84</v>
       </c>
@@ -33122,7 +33068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:49">
       <c r="A104" t="s">
         <v>85</v>
       </c>
@@ -33232,7 +33178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:49">
       <c r="A105" t="s">
         <v>85</v>
       </c>
@@ -33342,7 +33288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:49">
       <c r="A106" t="s">
         <v>85</v>
       </c>
@@ -33452,7 +33398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:49">
       <c r="A107" t="s">
         <v>85</v>
       </c>
@@ -33562,7 +33508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:49">
       <c r="A108" t="s">
         <v>86</v>
       </c>
@@ -33672,7 +33618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:49">
       <c r="A109" t="s">
         <v>86</v>
       </c>
@@ -33782,7 +33728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:49">
       <c r="A110" t="s">
         <v>86</v>
       </c>
@@ -33892,7 +33838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:49">
       <c r="A111" t="s">
         <v>86</v>
       </c>
@@ -34002,7 +33948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:49">
       <c r="A112" t="s">
         <v>87</v>
       </c>
@@ -34112,7 +34058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:49">
       <c r="A113" t="s">
         <v>87</v>
       </c>
@@ -34222,7 +34168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:49">
       <c r="A114" t="s">
         <v>87</v>
       </c>
@@ -34332,7 +34278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:49">
       <c r="A115" t="s">
         <v>88</v>
       </c>
@@ -34442,7 +34388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:49">
       <c r="A116" t="s">
         <v>88</v>
       </c>

</xml_diff>